<commit_message>
ch-lab-order 2.0.0 - ballot
</commit_message>
<xml_diff>
--- a/ig/ch-lab-order/CodeSystem-ServiceRequest.categories.xlsx
+++ b/ig/ch-lab-order/CodeSystem-ServiceRequest.categories.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Property</t>
   </si>
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://build.fhir.org/ig/hl7ch/ch-lab-order/CodeSystem/ServiceRequest.categories</t>
+    <t>http://fhir.ch/ig/ch-lab-order/CodeSystem/ServiceRequest.categories</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>2.0.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,6 +54,9 @@
     <t>Experimental</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -90,15 +93,12 @@
     <t>Copyright</t>
   </si>
   <si>
-    <t>CC-BY-SA-4.0</t>
+    <t>CC0-1.0</t>
   </si>
   <si>
     <t>Case Sensitive</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Value Set (all codes)</t>
   </si>
   <si>
@@ -123,7 +123,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>Level</t>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t>Electronic proposal for additional exam</t>
+  </si>
+  <si>
+    <t>RequestForHistopathExam</t>
+  </si>
+  <si>
+    <t>Anforderung von histopathologischen Untersuchungen</t>
+  </si>
+  <si>
+    <t>Electronic ordering of histopathologic tests and/or panels</t>
   </si>
 </sst>
 </file>
@@ -314,10 +323,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -326,7 +335,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -388,113 +397,123 @@
       <c r="A7" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>19</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s" s="2">
         <v>21</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="B14" t="s" s="2">
-        <v>25</v>
-      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s" s="2">
         <v>26</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>33</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
         <v>35</v>
       </c>
-      <c r="B22" t="s" s="2">
+      <c r="B23" t="s" s="2">
         <v>36</v>
       </c>
     </row>
@@ -505,7 +524,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -609,6 +628,20 @@
         <v>59</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>